<commit_message>
SELESAI SETELAH PERBAIKAN KECIL
</commit_message>
<xml_diff>
--- a/LAPORAN BUKU TAMU.xlsx
+++ b/LAPORAN BUKU TAMU.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
   <si>
     <t>NO</t>
   </si>
@@ -41,7 +41,34 @@
     <t>2025-09-07</t>
   </si>
   <si>
-    <t>Papay</t>
+    <t>Mega Siva Marhaeni</t>
+  </si>
+  <si>
+    <t>Kampung Babakan Sate</t>
+  </si>
+  <si>
+    <t>08080808</t>
+  </si>
+  <si>
+    <t>Nur Syifa Assawwala</t>
+  </si>
+  <si>
+    <t>Nyeblak di Teh Anna</t>
+  </si>
+  <si>
+    <t>Muhammad Haidar Almer Rafif</t>
+  </si>
+  <si>
+    <t>Perumahan Bumi Marhamah</t>
+  </si>
+  <si>
+    <t>085956267079</t>
+  </si>
+  <si>
+    <t>Presiden</t>
+  </si>
+  <si>
+    <t>Reformasi</t>
   </si>
 </sst>
 </file>
@@ -422,16 +449,16 @@
       <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2">
-        <v>12</v>
-      </c>
-      <c r="E2">
-        <v>12</v>
-      </c>
-      <c r="F2">
-        <v>12</v>
-      </c>
-      <c r="G2">
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
         <v>12</v>
       </c>
     </row>
@@ -443,19 +470,19 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>3</v>
-      </c>
-      <c r="G3">
-        <v>4</v>
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>